<commit_message>
Falta hacer andar lo de sergio Se agrego Conversion de Matriz a arreglo lineal
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -814,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:L34"/>
+  <dimension ref="C2:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="P81" sqref="P81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1016,7 +1016,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="6:9">
+    <row r="34" spans="6:15">
       <c r="F34" t="s">
         <v>8</v>
       </c>
@@ -1029,6 +1029,316 @@
       </c>
       <c r="I34" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="6:15">
+      <c r="O38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="6:15">
+      <c r="F39">
+        <v>3</v>
+      </c>
+      <c r="O39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="6:15">
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:15">
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="6:15">
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="6:15">
+      <c r="F43">
+        <v>3</v>
+      </c>
+      <c r="O43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="6:15">
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="6:15">
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="6:15">
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="O46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="6:15">
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="6:15">
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="6:15">
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="O49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="6:15">
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="6:15">
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="6:15">
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="O52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="6:15">
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="O53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="6:15">
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="6:15">
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="6:15">
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="6:15">
+      <c r="F57">
+        <v>4</v>
+      </c>
+      <c r="O57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="6:15">
+      <c r="F58">
+        <v>3</v>
+      </c>
+      <c r="O58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="6:15">
+      <c r="F59">
+        <v>4</v>
+      </c>
+      <c r="O59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="6:15">
+      <c r="F60">
+        <v>3</v>
+      </c>
+      <c r="O60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="6:15">
+      <c r="F61">
+        <v>5</v>
+      </c>
+      <c r="O61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="6:15">
+      <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="O62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="6:15">
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="O63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="6:15">
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="O64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="6:15">
+      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="6:15">
+      <c r="O66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="6:15">
+      <c r="F67">
+        <f>25*32*8*SUM(F39:F65)</f>
+        <v>396800</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="6:15">
+      <c r="O68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="6:15">
+      <c r="O69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="6:15">
+      <c r="O70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="6:15">
+      <c r="O71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="6:15">
+      <c r="O72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="6:15">
+      <c r="O73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="6:15">
+      <c r="O74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="6:15">
+      <c r="O75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="6:15">
+      <c r="O76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="6:15">
+      <c r="O77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="6:15">
+      <c r="O78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="6:15">
+      <c r="O79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="6:15">
+      <c r="O80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="15:16">
+      <c r="O81">
+        <f>SUM(O38:O80)</f>
+        <v>95</v>
+      </c>
+      <c r="P81">
+        <f>32*8*O81*25</f>
+        <v>608000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>